<commit_message>
Reworked the "Player" text in events as well.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B85321-AC74-4085-948B-3286393D9BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F5174E-4DB0-40F9-8048-691C0A9D63F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -250,13 +250,19 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>Player</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,13 +273,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -323,10 +322,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,10 +653,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -917,27 +916,35 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed "player" by "Player" in loc files.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F5174E-4DB0-40F9-8048-691C0A9D63F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C907ABAB-B351-4022-9C34-9EC2DED3C669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
   <si>
     <t>ID</t>
   </si>
@@ -252,10 +252,112 @@
     <t>None</t>
   </si>
   <si>
-    <t>player</t>
-  </si>
-  <si>
     <t>Player</t>
+  </si>
+  <si>
+    <t>SPANISH</t>
+  </si>
+  <si>
+    <t>Ninguno</t>
+  </si>
+  <si>
+    <t>Suelo</t>
+  </si>
+  <si>
+    <t>Suelo Cyan</t>
+  </si>
+  <si>
+    <t>Suelo Rojo</t>
+  </si>
+  <si>
+    <t>Suelo Naranja</t>
+  </si>
+  <si>
+    <t>Suelo Grande</t>
+  </si>
+  <si>
+    <t>Suelo 2</t>
+  </si>
+  <si>
+    <t>Pared</t>
+  </si>
+  <si>
+    <t>Pared Sin Color</t>
+  </si>
+  <si>
+    <t>Pared X</t>
+  </si>
+  <si>
+    <t>Ventana</t>
+  </si>
+  <si>
+    <t>Luz Direccional</t>
+  </si>
+  <si>
+    <t>Luz Puntual</t>
+  </si>
+  <si>
+    <t>Lámpara</t>
+  </si>
+  <si>
+    <t>Ventilación Verde</t>
+  </si>
+  <si>
+    <t>Ventilación Cyan</t>
+  </si>
+  <si>
+    <t>Paquete de Salud</t>
+  </si>
+  <si>
+    <t>Paquete de Munición</t>
+  </si>
+  <si>
+    <t>Sierra</t>
+  </si>
+  <si>
+    <t>Waypoint de Sierra</t>
+  </si>
+  <si>
+    <t>Interruptor</t>
+  </si>
+  <si>
+    <t>Spawn del Jugador</t>
+  </si>
+  <si>
+    <t>Cubo</t>
+  </si>
+  <si>
+    <t>Trampa de Fuego</t>
+  </si>
+  <si>
+    <t>Colisión</t>
+  </si>
+  <si>
+    <t>Trigger Final</t>
+  </si>
+  <si>
+    <t>Placa de Presión</t>
+  </si>
+  <si>
+    <t>Pantalla</t>
+  </si>
+  <si>
+    <t>Pantalla Pequeña</t>
+  </si>
+  <si>
+    <t>Ventana Frágil</t>
+  </si>
+  <si>
+    <t>Jugador</t>
+  </si>
+  <si>
+    <t>Cuando Se Activa</t>
+  </si>
+  <si>
+    <t>Cuando Se Desactiva</t>
+  </si>
+  <si>
+    <t>Cuando Se Invierte</t>
   </si>
 </sst>
 </file>
@@ -320,12 +422,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,312 +741,424 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
       <c r="B19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="B24" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>52</v>
       </c>
       <c r="B25" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
       <c r="B26" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
       <c r="B27" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
       <c r="B28" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
       <c r="B29" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>62</v>
       </c>
       <c r="B30" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>64</v>
       </c>
       <c r="B31" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>66</v>
       </c>
       <c r="B32" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
       <c r="B33" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added auto translations for category buttons.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DD927E-54F4-4F5D-95FC-EEEFE3B9207C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3860B07C-21AA-485C-8B40-252A2F31E725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="138">
   <si>
     <t>ID</t>
   </si>
@@ -403,6 +403,51 @@
   </si>
   <si>
     <t>On Exit</t>
+  </si>
+  <si>
+    <t>category.Structures</t>
+  </si>
+  <si>
+    <t>Structures</t>
+  </si>
+  <si>
+    <t>Estructuras</t>
+  </si>
+  <si>
+    <t>category.Decorations</t>
+  </si>
+  <si>
+    <t>Decorations</t>
+  </si>
+  <si>
+    <t>Decoraciones</t>
+  </si>
+  <si>
+    <t>category.Activables</t>
+  </si>
+  <si>
+    <t>Activables</t>
+  </si>
+  <si>
+    <t>Accionables</t>
+  </si>
+  <si>
+    <t>category.Traps</t>
+  </si>
+  <si>
+    <t>Traps</t>
+  </si>
+  <si>
+    <t>Trampas</t>
+  </si>
+  <si>
+    <t>category.System</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Sistema</t>
   </si>
 </sst>
 </file>
@@ -786,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,452 +857,507 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>119</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>118</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B47" t="s">
         <v>122</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C47" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added tootlip to set active at start toggle.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3860B07C-21AA-485C-8B40-252A2F31E725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912C24BC-6F56-4B9D-9449-1E8EB05B3758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="141">
   <si>
     <t>ID</t>
   </si>
@@ -448,6 +448,15 @@
   </si>
   <si>
     <t>Sistema</t>
+  </si>
+  <si>
+    <t>tooltip.SetActiveAtStartToggle</t>
+  </si>
+  <si>
+    <t>Define si el objeto estará [00FFFF]activado[-] o [FF0000]no[-] al inicio del nivel.</t>
+  </si>
+  <si>
+    <t>Defines if the object will be [00FFFF]enabled[-] or [FF0000]not[-] at the beginning of the level.</t>
   </si>
 </sst>
 </file>
@@ -512,10 +521,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,17 +849,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="2" max="3" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1279,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -1359,6 +1376,17 @@
       </c>
       <c r="C47" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organization and localization keys.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912C24BC-6F56-4B9D-9449-1E8EB05B3758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917DBA09-4051-4FBD-84A9-E7ED330D6B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="155">
   <si>
     <t>ID</t>
   </si>
@@ -457,6 +457,48 @@
   </si>
   <si>
     <t>Defines if the object will be [00FFFF]enabled[-] or [FF0000]not[-] at the beginning of the level.</t>
+  </si>
+  <si>
+    <t>pause.ExitPopup.Title</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Advertencia</t>
+  </si>
+  <si>
+    <t>pause.ExitPopup.Content</t>
+  </si>
+  <si>
+    <t>Advertencia, al salir se van a elimiar los cambios que hayas hecho desde el último guardado, ¿estás seguro de que deseas continuar?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>pause.ExitPopup.SaveAndExit</t>
+  </si>
+  <si>
+    <t>Save And Exit</t>
+  </si>
+  <si>
+    <t>Salir Y Guardar</t>
+  </si>
+  <si>
+    <t>pause.ExitPopup.ExitNoSave</t>
+  </si>
+  <si>
+    <t>Exit Without Saving</t>
+  </si>
+  <si>
+    <t>Salir Sin Guardar</t>
+  </si>
+  <si>
+    <t>pause.ExitPopup.Back</t>
+  </si>
+  <si>
+    <t>Warning, exiting will erase your last saved changes if you made any before saving, are you sure you want to continue?</t>
   </si>
 </sst>
 </file>
@@ -521,19 +563,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -849,532 +888,533 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="3" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" style="2" customWidth="1"/>
+    <col min="2" max="3" width="45.7109375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1382,11 +1422,66 @@
       <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="2" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fully translated LE pause menu.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917DBA09-4051-4FBD-84A9-E7ED330D6B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D95A23-08CB-4204-9900-4F7E5BC2081D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="170">
   <si>
     <t>ID</t>
   </si>
@@ -498,7 +498,52 @@
     <t>pause.ExitPopup.Back</t>
   </si>
   <si>
-    <t>Warning, exiting will erase your last saved changes if you made any before saving, are you sure you want to continue?</t>
+    <t>pause.PlayLevel</t>
+  </si>
+  <si>
+    <t>Play Level</t>
+  </si>
+  <si>
+    <t>Jugar Nivel</t>
+  </si>
+  <si>
+    <t>pause.SaveLevel</t>
+  </si>
+  <si>
+    <t>Save Level</t>
+  </si>
+  <si>
+    <t>Guardar Nivel</t>
+  </si>
+  <si>
+    <t>LevelEditor</t>
+  </si>
+  <si>
+    <t>Level Editor</t>
+  </si>
+  <si>
+    <t>Editor de Niveles</t>
+  </si>
+  <si>
+    <t>Warning, exiting now will delete any changes you have made since the last save. Are you sure you want to continue?</t>
+  </si>
+  <si>
+    <t>pause.NoSpawnObject</t>
+  </si>
+  <si>
+    <t>There isn't any player spawn obj in the scene.</t>
+  </si>
+  <si>
+    <t>No hay ningún spawn del jugador en la escena.</t>
+  </si>
+  <si>
+    <t>pause.NoChanges</t>
+  </si>
+  <si>
+    <t>There are no changes to save.</t>
+  </si>
+  <si>
+    <t>No hay cambios para guardar.</t>
   </si>
 </sst>
 </file>
@@ -888,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,573 +959,628 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added selected obj panel HEADER translations.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D95A23-08CB-4204-9900-4F7E5BC2081D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF62420-8D65-422B-8387-8CCF3310B2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="176">
   <si>
     <t>ID</t>
   </si>
@@ -544,6 +544,24 @@
   </si>
   <si>
     <t>No hay cambios para guardar.</t>
+  </si>
+  <si>
+    <t>No Object Selected</t>
+  </si>
+  <si>
+    <t>Sin Objeto Seleccionado</t>
+  </si>
+  <si>
+    <t>selection.NoObjectSelected</t>
+  </si>
+  <si>
+    <t>selection.MultipleObjectsSelected</t>
+  </si>
+  <si>
+    <t>Multiple Objects Selected</t>
+  </si>
+  <si>
+    <t>Multiples Objetos Seleccionados</t>
   </si>
 </sst>
 </file>
@@ -933,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,114 +1492,136 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>140</v>
+        <v>154</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>152</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added translations for global attributes.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF62420-8D65-422B-8387-8CCF3310B2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D411AC3-D2E7-4053-A1CD-AFCE5BE6F27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -562,6 +562,24 @@
   </si>
   <si>
     <t>Multiples Objetos Seleccionados</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Posición</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
+    <t>Rotación</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Escala</t>
   </si>
 </sst>
 </file>
@@ -951,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,14 +1631,47 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added FULLY translations for the Selected Obj Panel :)
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D411AC3-D2E7-4053-A1CD-AFCE5BE6F27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF97210-427A-4B42-B9C4-64BFCFB8B69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="248">
   <si>
     <t>ID</t>
   </si>
@@ -580,6 +580,204 @@
   </si>
   <si>
     <t>Escala</t>
+  </si>
+  <si>
+    <t>ColorHex</t>
+  </si>
+  <si>
+    <t>Color (Hex)</t>
+  </si>
+  <si>
+    <t>Intensity</t>
+  </si>
+  <si>
+    <t>Intensidad</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>ActivateOnStart</t>
+  </si>
+  <si>
+    <t>Activate On Start</t>
+  </si>
+  <si>
+    <t>Activar Al Inicio</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Daño</t>
+  </si>
+  <si>
+    <t>TravelBack</t>
+  </si>
+  <si>
+    <t>Travel Back</t>
+  </si>
+  <si>
+    <t>Regresarse</t>
+  </si>
+  <si>
+    <t>AddWaypoint</t>
+  </si>
+  <si>
+    <t>+ Add Waypoint</t>
+  </si>
+  <si>
+    <t>+ Añadir Waypoint</t>
+  </si>
+  <si>
+    <t>WaitTime</t>
+  </si>
+  <si>
+    <t>Wait Time</t>
+  </si>
+  <si>
+    <t>Tiempo de Espera</t>
+  </si>
+  <si>
+    <t>InitialState</t>
+  </si>
+  <si>
+    <t>Initial State</t>
+  </si>
+  <si>
+    <t>Estado Inicial</t>
+  </si>
+  <si>
+    <t>DEACTIVATED</t>
+  </si>
+  <si>
+    <t>DESACTIVADO</t>
+  </si>
+  <si>
+    <t>ACTIVATED</t>
+  </si>
+  <si>
+    <t>ACTIVADO</t>
+  </si>
+  <si>
+    <t>UNUSABLE</t>
+  </si>
+  <si>
+    <t>UsableOnce</t>
+  </si>
+  <si>
+    <t>Usable Once</t>
+  </si>
+  <si>
+    <t>Usable Una Vez</t>
+  </si>
+  <si>
+    <t>CanBeShotByTaser</t>
+  </si>
+  <si>
+    <t>Can be shot by Taser</t>
+  </si>
+  <si>
+    <t>Puede ser activado por el Taser</t>
+  </si>
+  <si>
+    <t>ManageEvents</t>
+  </si>
+  <si>
+    <t>Manage Events</t>
+  </si>
+  <si>
+    <t>Administrar Eventos</t>
+  </si>
+  <si>
+    <t>RespawnTime</t>
+  </si>
+  <si>
+    <t>Respawn Time</t>
+  </si>
+  <si>
+    <t>Tiempo de Reaparición</t>
+  </si>
+  <si>
+    <t>Muerte Instantanea</t>
+  </si>
+  <si>
+    <t>Instant Kill</t>
+  </si>
+  <si>
+    <t>InstantKill</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Constante</t>
+  </si>
+  <si>
+    <t>OnlyOnce</t>
+  </si>
+  <si>
+    <t>Only Once</t>
+  </si>
+  <si>
+    <t>Una sola Vez</t>
+  </si>
+  <si>
+    <t>ScreenColor</t>
+  </si>
+  <si>
+    <t>Screen Color</t>
+  </si>
+  <si>
+    <t>Color de la Pantalla</t>
+  </si>
+  <si>
+    <t>CYAN</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>ROJO</t>
+  </si>
+  <si>
+    <t>InvisibleMesh</t>
+  </si>
+  <si>
+    <t>Invisible Mesh</t>
+  </si>
+  <si>
+    <t>Malla Invisible</t>
+  </si>
+  <si>
+    <t>InvertTextWithGravity</t>
+  </si>
+  <si>
+    <t>Invert Text With Gravity</t>
+  </si>
+  <si>
+    <t>Invertir Texto Con La Gravedad</t>
+  </si>
+  <si>
+    <t>EditText</t>
+  </si>
+  <si>
+    <t>Edit Text</t>
+  </si>
+  <si>
+    <t>Editar Texto</t>
+  </si>
+  <si>
+    <t>Collision</t>
   </si>
 </sst>
 </file>
@@ -644,7 +842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -654,6 +852,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,18 +1865,316 @@
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added translation for the current mode label.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF97210-427A-4B42-B9C4-64BFCFB8B69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1577CE9E-CD7D-49D5-B46B-BCE72E28BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="257">
   <si>
     <t>ID</t>
   </si>
@@ -778,6 +778,33 @@
   </si>
   <si>
     <t>Collision</t>
+  </si>
+  <si>
+    <t>CurrentMode</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Construcción</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>Selección</t>
+  </si>
+  <si>
+    <t>Deletion</t>
+  </si>
+  <si>
+    <t>Eliminación</t>
+  </si>
+  <si>
+    <t>[c][ffff00]Modo Actual:[-][/c]</t>
+  </si>
+  <si>
+    <t>[c][ffff00]Current Mode:[-][/c]</t>
   </si>
 </sst>
 </file>
@@ -1170,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,6 +2200,50 @@
         <v>246</v>
       </c>
     </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added FULLY translations for Global Properties panel.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1577CE9E-CD7D-49D5-B46B-BCE72E28BF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E828892-48D3-48E7-818A-DB56EF2B55D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="276">
   <si>
     <t>ID</t>
   </si>
@@ -805,13 +805,70 @@
   </si>
   <si>
     <t>[c][ffff00]Current Mode:[-][/c]</t>
+  </si>
+  <si>
+    <t>GlobalProperties</t>
+  </si>
+  <si>
+    <t>Global Properties</t>
+  </si>
+  <si>
+    <t>Propiedades Globales</t>
+  </si>
+  <si>
+    <t>HasTaser</t>
+  </si>
+  <si>
+    <t>Has Taser</t>
+  </si>
+  <si>
+    <t>Con Taser</t>
+  </si>
+  <si>
+    <t>HasJetpack</t>
+  </si>
+  <si>
+    <t>Has Jetpack</t>
+  </si>
+  <si>
+    <t>Con Jetpack</t>
+  </si>
+  <si>
+    <t>DeathYLimit</t>
+  </si>
+  <si>
+    <t>Death Limit on the Y-axis</t>
+  </si>
+  <si>
+    <t>Límite de Muerte en el eje Y</t>
+  </si>
+  <si>
+    <t>Skybox</t>
+  </si>
+  <si>
+    <t>Chapter 1</t>
+  </si>
+  <si>
+    <t>Capítulo 1</t>
+  </si>
+  <si>
+    <t>Chapter 2</t>
+  </si>
+  <si>
+    <t>Capítulo 2</t>
+  </si>
+  <si>
+    <t>Chapter 3 &amp; 4</t>
+  </si>
+  <si>
+    <t>Capítulo 3 &amp; 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,6 +880,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1197,10 +1260,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
-  <dimension ref="A1:C94"/>
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2244,7 +2308,96 @@
         <v>254</v>
       </c>
     </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Forgot to add Loop translations LOL.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E828892-48D3-48E7-818A-DB56EF2B55D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A530195-FF47-41F5-9CE0-1F29D6572013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="278">
   <si>
     <t>ID</t>
   </si>
@@ -861,7 +861,13 @@
     <t>Chapter 3 &amp; 4</t>
   </si>
   <si>
-    <t>Capítulo 3 &amp; 4</t>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>Bucle</t>
+  </si>
+  <si>
+    <t>Capítulo 3 Y 4</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1267,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,7 +2399,18 @@
         <v>274</v>
       </c>
       <c r="C102" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>275</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tooltips for the saw toggles.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A530195-FF47-41F5-9CE0-1F29D6572013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E337775-75A0-4681-8BE5-827679C7D3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="284">
   <si>
     <t>ID</t>
   </si>
@@ -868,6 +868,24 @@
   </si>
   <si>
     <t>Capítulo 3 Y 4</t>
+  </si>
+  <si>
+    <t>TravelBackTooltip</t>
+  </si>
+  <si>
+    <t>LoopTooltip</t>
+  </si>
+  <si>
+    <t>The saw [00FFFF]returns[-] to its original position by [FFFF00]passing through the waypoints.[-]</t>
+  </si>
+  <si>
+    <t>The saw [00FFFF]returns[-] to its original position in a [FFFF00]straight line [b]ignoring[/b] the waypoints.[-]</t>
+  </si>
+  <si>
+    <t>La sierra [00FFFF]regresa[-] a su posición original en una [FFFF00]linea recta [b]ignorando[/b] los waypoints.[-]</t>
+  </si>
+  <si>
+    <t>La sierra [00FFFF]regresa[-] a su posición original al [FFFF00]pasar por todos sus waypoints.[-]</t>
   </si>
 </sst>
 </file>
@@ -1267,10 +1285,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,6 +2431,28 @@
         <v>276</v>
       </c>
     </row>
+    <row r="104" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Door V2 translation in the sheet.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC7F990-A075-460D-BA01-33A2672DF931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EE1F2C-4A6E-45BB-A09F-E77BAD11F960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="293">
   <si>
     <t>ID</t>
   </si>
@@ -904,6 +904,15 @@
   </si>
   <si>
     <t>Campo Laser</t>
+  </si>
+  <si>
+    <t>object.DOOR_V2</t>
+  </si>
+  <si>
+    <t>Door V2</t>
+  </si>
+  <si>
+    <t>Puerta V2</t>
   </si>
 </sst>
 </file>
@@ -1303,10 +1312,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,727 +1778,738 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>69</v>
+        <v>290</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>69</v>
+        <v>291</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>101</v>
+        <v>292</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="50" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+    <row r="57" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+    <row r="107" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>282</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a tooltip for the door state button in events panel.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EE1F2C-4A6E-45BB-A09F-E77BAD11F960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECB8F3B-F024-4465-AE9E-59EA58FA17E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="296">
   <si>
     <t>ID</t>
   </si>
@@ -913,6 +913,15 @@
   </si>
   <si>
     <t>Puerta V2</t>
+  </si>
+  <si>
+    <t>EventsDoorStateTooltip</t>
+  </si>
+  <si>
+    <t>[b][FFFF00]NOTE:[-][/b] If the door is set as [00FFFF]automatic[-], trying to open it will only [b]allow it to open[/b], but it won't really open until a [b]player gets closer to it.[/b]</t>
+  </si>
+  <si>
+    <t>[b][FFFF00]NOTA:[-][/b] Si la puerta está puesta como [00FFFF]automática[-], tratar de abrirla solo le [b]permitirá abrirse[/b], pero no se abrirá realmente hasta que [b]el jugador se acerque a ella.[/b]</t>
   </si>
 </sst>
 </file>
@@ -1312,10 +1321,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,6 +2522,17 @@
         <v>282</v>
       </c>
     </row>
+    <row r="109" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added translation for "Scaled Text"
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40F82F1-81D3-421E-96D2-8BEC945E4CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09EC387C-9623-4E54-8E7A-21F67C18C693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="307">
   <si>
     <t>ID</t>
   </si>
@@ -946,6 +946,15 @@
   </si>
   <si>
     <t>Duración Prendido</t>
+  </si>
+  <si>
+    <t>ScaledText</t>
+  </si>
+  <si>
+    <t>Scaled Text</t>
+  </si>
+  <si>
+    <t>Texto Escalado</t>
   </si>
 </sst>
 </file>
@@ -1345,10 +1354,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,188 +2414,199 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>244</v>
+        <v>304</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>245</v>
+        <v>305</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>246</v>
+        <v>306</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+    <row r="112" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C112" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+    <row r="113" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>295</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made the flame trap throw cubes harder, scaling Chris suggested and added Saw rotation (although glitched when hitting the first/last waypoint, your fault, not mine)
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\c#\FrSLE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB04E67A-D435-4D4E-AB82-04BA9978556A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAC4CB9-C537-4337-9354-6087E4787E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15900" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="439">
   <si>
     <t>ID</t>
   </si>
@@ -997,6 +997,360 @@
   </si>
   <si>
     <t>Retraso</t>
+  </si>
+  <si>
+    <t>Rotate</t>
+  </si>
+  <si>
+    <t>Rotate?</t>
+  </si>
+  <si>
+    <t>RotateSpeed</t>
+  </si>
+  <si>
+    <t>Rotate speed</t>
+  </si>
+  <si>
+    <t>UKRAINIAN</t>
+  </si>
+  <si>
+    <t>Редактор</t>
+  </si>
+  <si>
+    <t>Структури</t>
+  </si>
+  <si>
+    <t>Декорації</t>
+  </si>
+  <si>
+    <t>Активуваньці</t>
+  </si>
+  <si>
+    <t>Пастки</t>
+  </si>
+  <si>
+    <t>Система</t>
+  </si>
+  <si>
+    <t>Ніякий</t>
+  </si>
+  <si>
+    <t>Підлога</t>
+  </si>
+  <si>
+    <t>Голуба підлога</t>
+  </si>
+  <si>
+    <t>Червона підлога</t>
+  </si>
+  <si>
+    <t>Оранжева підлога</t>
+  </si>
+  <si>
+    <t>Велика підлога</t>
+  </si>
+  <si>
+    <t>Підлога 2</t>
+  </si>
+  <si>
+    <t>Стіна</t>
+  </si>
+  <si>
+    <t>Стіна без кольору</t>
+  </si>
+  <si>
+    <t>Стіна Х</t>
+  </si>
+  <si>
+    <t>Вікно</t>
+  </si>
+  <si>
+    <t>Направлене світло</t>
+  </si>
+  <si>
+    <t>Точкове світло</t>
+  </si>
+  <si>
+    <t>Стельове світло</t>
+  </si>
+  <si>
+    <t>Вентиляція з зеленим димом</t>
+  </si>
+  <si>
+    <t>Вентиляція з голубим димом</t>
+  </si>
+  <si>
+    <t>Аптечка</t>
+  </si>
+  <si>
+    <t>Патрони</t>
+  </si>
+  <si>
+    <t>Пила</t>
+  </si>
+  <si>
+    <t>Проміжна точка пили</t>
+  </si>
+  <si>
+    <t>Перемикач</t>
+  </si>
+  <si>
+    <t>Місце появи гравця</t>
+  </si>
+  <si>
+    <t>Куб</t>
+  </si>
+  <si>
+    <t>Лазер</t>
+  </si>
+  <si>
+    <t>Вогнева пастка</t>
+  </si>
+  <si>
+    <t>Невидима стіна</t>
+  </si>
+  <si>
+    <t>Кінець</t>
+  </si>
+  <si>
+    <t>Нажимна плита</t>
+  </si>
+  <si>
+    <t>Екран</t>
+  </si>
+  <si>
+    <t>Малий екран</t>
+  </si>
+  <si>
+    <t>Крихке скло</t>
+  </si>
+  <si>
+    <t>Трігер</t>
+  </si>
+  <si>
+    <t>Двері</t>
+  </si>
+  <si>
+    <t>Лазерне поле</t>
+  </si>
+  <si>
+    <t>Двері V2</t>
+  </si>
+  <si>
+    <t>Трігер смерті</t>
+  </si>
+  <si>
+    <t>Гравець</t>
+  </si>
+  <si>
+    <t>Коли активне</t>
+  </si>
+  <si>
+    <t>Коли неактивне</t>
+  </si>
+  <si>
+    <t>Коли навпаки</t>
+  </si>
+  <si>
+    <t>На обох</t>
+  </si>
+  <si>
+    <t>При вході</t>
+  </si>
+  <si>
+    <t>При виході</t>
+  </si>
+  <si>
+    <t>Грати рівень</t>
+  </si>
+  <si>
+    <t>В сцені немає точки появи гравця.</t>
+  </si>
+  <si>
+    <t>Зберегти рівень</t>
+  </si>
+  <si>
+    <t>Немає змін, щоб зберегти.</t>
+  </si>
+  <si>
+    <t>Попередження</t>
+  </si>
+  <si>
+    <t>Попередження, якщо зараз вийти, то весь прогрес з минулого збереження буде втрачено. Ви впевнені, що хочете продовжити?</t>
+  </si>
+  <si>
+    <t>Вийти та зберегти</t>
+  </si>
+  <si>
+    <t>Вийти без збереження</t>
+  </si>
+  <si>
+    <t>Немає активного об'єкту</t>
+  </si>
+  <si>
+    <t>Декілька об'єктів вибрано</t>
+  </si>
+  <si>
+    <t>Позиція</t>
+  </si>
+  <si>
+    <t>Поворот</t>
+  </si>
+  <si>
+    <t>Розмір</t>
+  </si>
+  <si>
+    <t>Колізія</t>
+  </si>
+  <si>
+    <t>Вирішує, чи об'єкт буде [00FFFF]активний[-] чи [FF0000]ні[-] на початку рівня.</t>
+  </si>
+  <si>
+    <t>Колір (Hex)</t>
+  </si>
+  <si>
+    <t>Інтенсивність</t>
+  </si>
+  <si>
+    <t>Діапазон</t>
+  </si>
+  <si>
+    <t>Активувати на старті</t>
+  </si>
+  <si>
+    <t>Шкода</t>
+  </si>
+  <si>
+    <t>Повернутись назад</t>
+  </si>
+  <si>
+    <t>Час очікування</t>
+  </si>
+  <si>
+    <t>"+ додати проміжну точку"</t>
+  </si>
+  <si>
+    <t>Початковий стан</t>
+  </si>
+  <si>
+    <t>ДЕАКТИВОВАНИЙ</t>
+  </si>
+  <si>
+    <t>АКТИВОВАНИЙ</t>
+  </si>
+  <si>
+    <t>НЕДОСТУПНИЙ</t>
+  </si>
+  <si>
+    <t>Доступний один раз</t>
+  </si>
+  <si>
+    <t>Можна активувати тазером</t>
+  </si>
+  <si>
+    <t>Керувати подіями</t>
+  </si>
+  <si>
+    <t>Час відновлення</t>
+  </si>
+  <si>
+    <t>Моментальна смерть</t>
+  </si>
+  <si>
+    <t>Мигання</t>
+  </si>
+  <si>
+    <t>Тривалість ON</t>
+  </si>
+  <si>
+    <t>Тривалість OFF</t>
+  </si>
+  <si>
+    <t>Постійне</t>
+  </si>
+  <si>
+    <t>Лише раз</t>
+  </si>
+  <si>
+    <t>Колір екрану</t>
+  </si>
+  <si>
+    <t>Голубий</t>
+  </si>
+  <si>
+    <t>Зелений</t>
+  </si>
+  <si>
+    <t>Червоний</t>
+  </si>
+  <si>
+    <t>Невидимий екран</t>
+  </si>
+  <si>
+    <t>Перевертати текст з гравітацією</t>
+  </si>
+  <si>
+    <t>Розмір тексту</t>
+  </si>
+  <si>
+    <t>Редагувати текст</t>
+  </si>
+  <si>
+    <t>[c][ffff00]Поточний режим:[-][/c]</t>
+  </si>
+  <si>
+    <t>Будівництво</t>
+  </si>
+  <si>
+    <t>Вибір</t>
+  </si>
+  <si>
+    <t>Видалення</t>
+  </si>
+  <si>
+    <t>Глобальні настройки</t>
+  </si>
+  <si>
+    <t>Має тазер</t>
+  </si>
+  <si>
+    <t>Має джетпак</t>
+  </si>
+  <si>
+    <t>Ліміт по осі Y для смерті</t>
+  </si>
+  <si>
+    <t>Скайбокс</t>
+  </si>
+  <si>
+    <t>Глава 1</t>
+  </si>
+  <si>
+    <t>Глава 2</t>
+  </si>
+  <si>
+    <t>Глава 3 &amp; 4</t>
+  </si>
+  <si>
+    <t>Цикл</t>
+  </si>
+  <si>
+    <t>Тип</t>
+  </si>
+  <si>
+    <t>РЕЛОКАЦІЯ</t>
+  </si>
+  <si>
+    <t>СМЕРТЬ</t>
+  </si>
+  <si>
+    <t>Затримка</t>
+  </si>
+  <si>
+    <t>Повертати?</t>
+  </si>
+  <si>
+    <t>Швидкість повертання</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1081,12 +1435,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1102,9 +1453,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема &quot;Office 2013 – 2022&quot;">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1142,7 +1493,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1248,7 +1599,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1390,7 +1741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1399,20 +1750,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:C122"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="45.7109375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="2"/>
+    <col min="2" max="4" width="45.7109375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1422,8 +1773,11 @@
       <c r="C1" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>160</v>
       </c>
@@ -1433,8 +1787,11 @@
       <c r="C2" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>123</v>
       </c>
@@ -1444,8 +1801,11 @@
       <c r="C3" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>126</v>
       </c>
@@ -1455,8 +1815,11 @@
       <c r="C4" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>129</v>
       </c>
@@ -1466,8 +1829,11 @@
       <c r="C5" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>132</v>
       </c>
@@ -1477,8 +1843,11 @@
       <c r="C6" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>135</v>
       </c>
@@ -1488,8 +1857,11 @@
       <c r="C7" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>67</v>
       </c>
@@ -1499,8 +1871,11 @@
       <c r="C8" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1510,8 +1885,11 @@
       <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -1521,8 +1899,11 @@
       <c r="C10" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1532,8 +1913,11 @@
       <c r="C11" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1543,8 +1927,11 @@
       <c r="C12" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1554,8 +1941,11 @@
       <c r="C13" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1565,8 +1955,11 @@
       <c r="C14" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1576,8 +1969,11 @@
       <c r="C15" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1587,8 +1983,11 @@
       <c r="C16" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1598,8 +1997,11 @@
       <c r="C17" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1609,8 +2011,11 @@
       <c r="C18" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1620,8 +2025,11 @@
       <c r="C19" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1631,8 +2039,11 @@
       <c r="C20" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1642,8 +2053,11 @@
       <c r="C21" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
@@ -1653,8 +2067,11 @@
       <c r="C22" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -1664,8 +2081,11 @@
       <c r="C23" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
@@ -1675,8 +2095,11 @@
       <c r="C24" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -1686,8 +2109,11 @@
       <c r="C25" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -1697,8 +2123,11 @@
       <c r="C26" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>41</v>
       </c>
@@ -1708,8 +2137,11 @@
       <c r="C27" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
@@ -1719,8 +2151,11 @@
       <c r="C28" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -1730,8 +2165,11 @@
       <c r="C29" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>47</v>
       </c>
@@ -1741,8 +2179,11 @@
       <c r="C30" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
@@ -1752,8 +2193,11 @@
       <c r="C31" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
@@ -1763,8 +2207,11 @@
       <c r="C32" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>53</v>
       </c>
@@ -1774,8 +2221,11 @@
       <c r="C33" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>55</v>
       </c>
@@ -1785,8 +2235,11 @@
       <c r="C34" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>57</v>
       </c>
@@ -1796,8 +2249,11 @@
       <c r="C35" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>59</v>
       </c>
@@ -1807,8 +2263,11 @@
       <c r="C36" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>61</v>
       </c>
@@ -1818,8 +2277,11 @@
       <c r="C37" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>63</v>
       </c>
@@ -1829,8 +2291,11 @@
       <c r="C38" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>65</v>
       </c>
@@ -1840,8 +2305,11 @@
       <c r="C39" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>284</v>
       </c>
@@ -1851,8 +2319,11 @@
       <c r="C40" s="2" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>287</v>
       </c>
@@ -1862,8 +2333,11 @@
       <c r="C41" s="2" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>290</v>
       </c>
@@ -1873,8 +2347,11 @@
       <c r="C42" s="2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>307</v>
       </c>
@@ -1884,8 +2361,11 @@
       <c r="C43" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>69</v>
       </c>
@@ -1895,8 +2375,11 @@
       <c r="C44" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>105</v>
       </c>
@@ -1906,8 +2389,11 @@
       <c r="C45" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>106</v>
       </c>
@@ -1917,8 +2403,11 @@
       <c r="C46" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>107</v>
       </c>
@@ -1928,8 +2417,11 @@
       <c r="C47" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>108</v>
       </c>
@@ -1939,8 +2431,11 @@
       <c r="C48" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>110</v>
       </c>
@@ -1950,8 +2445,11 @@
       <c r="C49" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>114</v>
       </c>
@@ -1961,8 +2459,11 @@
       <c r="C50" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>117</v>
       </c>
@@ -1972,8 +2473,11 @@
       <c r="C51" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>118</v>
       </c>
@@ -1983,8 +2487,11 @@
       <c r="C52" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>154</v>
       </c>
@@ -1994,8 +2501,11 @@
       <c r="C53" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>164</v>
       </c>
@@ -2005,8 +2515,11 @@
       <c r="C54" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>157</v>
       </c>
@@ -2016,8 +2529,11 @@
       <c r="C55" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>167</v>
       </c>
@@ -2027,8 +2543,11 @@
       <c r="C56" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>141</v>
       </c>
@@ -2038,8 +2557,11 @@
       <c r="C57" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>144</v>
       </c>
@@ -2049,8 +2571,11 @@
       <c r="C58" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>153</v>
       </c>
@@ -2060,8 +2585,11 @@
       <c r="C59" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>147</v>
       </c>
@@ -2071,8 +2599,11 @@
       <c r="C60" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>150</v>
       </c>
@@ -2082,8 +2613,11 @@
       <c r="C61" s="2" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>172</v>
       </c>
@@ -2093,8 +2627,11 @@
       <c r="C62" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>173</v>
       </c>
@@ -2104,8 +2641,11 @@
       <c r="C63" s="2" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>176</v>
       </c>
@@ -2115,8 +2655,11 @@
       <c r="C64" s="2" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>178</v>
       </c>
@@ -2126,8 +2669,11 @@
       <c r="C65" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>180</v>
       </c>
@@ -2137,8 +2683,11 @@
       <c r="C66" s="2" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>247</v>
       </c>
@@ -2148,8 +2697,11 @@
       <c r="C67" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>138</v>
       </c>
@@ -2159,8 +2711,11 @@
       <c r="C68" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>182</v>
       </c>
@@ -2170,8 +2725,11 @@
       <c r="C69" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>184</v>
       </c>
@@ -2181,8 +2739,11 @@
       <c r="C70" s="2" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>186</v>
       </c>
@@ -2192,8 +2753,11 @@
       <c r="C71" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>188</v>
       </c>
@@ -2203,8 +2767,11 @@
       <c r="C72" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>191</v>
       </c>
@@ -2214,8 +2781,11 @@
       <c r="C73" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>193</v>
       </c>
@@ -2225,8 +2795,11 @@
       <c r="C74" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>196</v>
       </c>
@@ -2236,8 +2809,11 @@
       <c r="C75" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>199</v>
       </c>
@@ -2247,8 +2823,11 @@
       <c r="C76" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>202</v>
       </c>
@@ -2258,8 +2837,11 @@
       <c r="C77" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>205</v>
       </c>
@@ -2269,8 +2851,11 @@
       <c r="C78" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>207</v>
       </c>
@@ -2280,8 +2865,11 @@
       <c r="C79" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>209</v>
       </c>
@@ -2291,8 +2879,11 @@
       <c r="C80" s="2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>210</v>
       </c>
@@ -2302,8 +2893,11 @@
       <c r="C81" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>213</v>
       </c>
@@ -2313,8 +2907,11 @@
       <c r="C82" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>216</v>
       </c>
@@ -2324,8 +2921,11 @@
       <c r="C83" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>219</v>
       </c>
@@ -2335,8 +2935,11 @@
       <c r="C84" s="2" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>224</v>
       </c>
@@ -2346,8 +2949,11 @@
       <c r="C85" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>296</v>
       </c>
@@ -2357,8 +2963,11 @@
       <c r="C86" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>298</v>
       </c>
@@ -2368,8 +2977,11 @@
       <c r="C87" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>301</v>
       </c>
@@ -2379,8 +2991,11 @@
       <c r="C88" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>225</v>
       </c>
@@ -2390,8 +3005,11 @@
       <c r="C89" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>227</v>
       </c>
@@ -2401,8 +3019,11 @@
       <c r="C90" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>230</v>
       </c>
@@ -2412,8 +3033,11 @@
       <c r="C91" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>233</v>
       </c>
@@ -2423,8 +3047,11 @@
       <c r="C92" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>234</v>
       </c>
@@ -2434,8 +3061,11 @@
       <c r="C93" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>236</v>
       </c>
@@ -2445,8 +3075,11 @@
       <c r="C94" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>238</v>
       </c>
@@ -2456,8 +3089,11 @@
       <c r="C95" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>241</v>
       </c>
@@ -2467,8 +3103,11 @@
       <c r="C96" s="2" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>304</v>
       </c>
@@ -2478,8 +3117,11 @@
       <c r="C97" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>244</v>
       </c>
@@ -2489,8 +3131,11 @@
       <c r="C98" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>248</v>
       </c>
@@ -2500,8 +3145,11 @@
       <c r="C99" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>249</v>
       </c>
@@ -2511,8 +3159,11 @@
       <c r="C100" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>251</v>
       </c>
@@ -2522,8 +3173,11 @@
       <c r="C101" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>253</v>
       </c>
@@ -2533,8 +3187,11 @@
       <c r="C102" s="2" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>257</v>
       </c>
@@ -2544,8 +3201,11 @@
       <c r="C103" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>260</v>
       </c>
@@ -2555,8 +3215,11 @@
       <c r="C104" s="2" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>263</v>
       </c>
@@ -2566,8 +3229,11 @@
       <c r="C105" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>266</v>
       </c>
@@ -2577,8 +3243,11 @@
       <c r="C106" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>269</v>
       </c>
@@ -2588,8 +3257,11 @@
       <c r="C107" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>270</v>
       </c>
@@ -2599,8 +3271,11 @@
       <c r="C108" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>272</v>
       </c>
@@ -2610,8 +3285,11 @@
       <c r="C109" s="2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>274</v>
       </c>
@@ -2621,8 +3299,11 @@
       <c r="C110" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>275</v>
       </c>
@@ -2632,8 +3313,11 @@
       <c r="C111" s="2" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>278</v>
       </c>
@@ -2644,7 +3328,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>279</v>
       </c>
@@ -2655,7 +3339,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>293</v>
       </c>
@@ -2666,7 +3350,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>310</v>
       </c>
@@ -2676,8 +3360,11 @@
       <c r="C115" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>313</v>
       </c>
@@ -2687,8 +3374,11 @@
       <c r="C116" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>314</v>
       </c>
@@ -2698,8 +3388,11 @@
       <c r="C117" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>319</v>
       </c>
@@ -2709,9 +3402,31 @@
       <c r="C118" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B122" s="5"/>
+      <c r="D118" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>438</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Changed the translations for "Add Waypoint", added two more instead (Gray, I had to delete your translation, but only that one).
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\c#\FrSLE\Translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAC4CB9-C537-4337-9354-6087E4787E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251A6008-6540-445F-9852-48FA855F7E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15900" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="441">
   <si>
     <t>ID</t>
   </si>
@@ -624,15 +624,6 @@
     <t>Regresarse</t>
   </si>
   <si>
-    <t>AddWaypoint</t>
-  </si>
-  <si>
-    <t>+ Add Waypoint</t>
-  </si>
-  <si>
-    <t>+ Añadir Waypoint</t>
-  </si>
-  <si>
     <t>WaitTime</t>
   </si>
   <si>
@@ -1227,9 +1218,6 @@
     <t>Час очікування</t>
   </si>
   <si>
-    <t>"+ додати проміжну точку"</t>
-  </si>
-  <si>
     <t>Початковий стан</t>
   </si>
   <si>
@@ -1351,6 +1339,24 @@
   </si>
   <si>
     <t>Швидкість повертання</t>
+  </si>
+  <si>
+    <t>AddGlobalWaypoint</t>
+  </si>
+  <si>
+    <t>+ Add Global Waypoint</t>
+  </si>
+  <si>
+    <t>+ Añadir Waypoint Global</t>
+  </si>
+  <si>
+    <t>AddSawWaypoint</t>
+  </si>
+  <si>
+    <t>+ Add Saw Waypoint</t>
+  </si>
+  <si>
+    <t>+ Añadir Waypoint de Sierra</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1443,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1453,9 +1459,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема &quot;Office 2013 – 2022&quot;">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013–2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1493,7 +1499,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013–2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1599,7 +1605,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013–2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1741,7 +1747,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1750,13 +1756,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" style="2" customWidth="1"/>
     <col min="2" max="4" width="45.7109375" style="2" customWidth="1"/>
@@ -1774,7 +1780,7 @@
         <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1788,7 +1794,7 @@
         <v>162</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1802,7 +1808,7 @@
         <v>125</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1816,7 +1822,7 @@
         <v>128</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1830,7 +1836,7 @@
         <v>131</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1844,7 +1850,7 @@
         <v>134</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1858,7 +1864,7 @@
         <v>137</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1872,7 +1878,7 @@
         <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1886,7 +1892,7 @@
         <v>72</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1900,7 +1906,7 @@
         <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1914,7 +1920,7 @@
         <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1928,7 +1934,7 @@
         <v>75</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1942,7 +1948,7 @@
         <v>76</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1956,7 +1962,7 @@
         <v>77</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1970,7 +1976,7 @@
         <v>78</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1984,7 +1990,7 @@
         <v>79</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1998,7 +2004,7 @@
         <v>80</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2012,7 +2018,7 @@
         <v>81</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2026,7 +2032,7 @@
         <v>82</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2040,7 +2046,7 @@
         <v>83</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2054,7 +2060,7 @@
         <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2068,7 +2074,7 @@
         <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2082,7 +2088,7 @@
         <v>86</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2096,7 +2102,7 @@
         <v>87</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2110,7 +2116,7 @@
         <v>88</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2124,7 +2130,7 @@
         <v>89</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2138,7 +2144,7 @@
         <v>90</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2152,7 +2158,7 @@
         <v>91</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2166,7 +2172,7 @@
         <v>92</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2180,7 +2186,7 @@
         <v>93</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2194,7 +2200,7 @@
         <v>50</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2208,7 +2214,7 @@
         <v>94</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2222,7 +2228,7 @@
         <v>95</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2236,7 +2242,7 @@
         <v>96</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2250,7 +2256,7 @@
         <v>97</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2264,7 +2270,7 @@
         <v>98</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2278,7 +2284,7 @@
         <v>99</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2292,7 +2298,7 @@
         <v>100</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2306,63 +2312,63 @@
         <v>66</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,7 +2382,7 @@
         <v>101</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2390,7 +2396,7 @@
         <v>102</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2404,7 +2410,7 @@
         <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2418,7 +2424,7 @@
         <v>104</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2432,7 +2438,7 @@
         <v>109</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2446,7 +2452,7 @@
         <v>113</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2460,7 +2466,7 @@
         <v>116</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2474,7 +2480,7 @@
         <v>120</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2488,7 +2494,7 @@
         <v>121</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2502,7 +2508,7 @@
         <v>156</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2516,7 +2522,7 @@
         <v>166</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2530,7 +2536,7 @@
         <v>159</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2544,7 +2550,7 @@
         <v>169</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2558,7 +2564,7 @@
         <v>143</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2572,7 +2578,7 @@
         <v>145</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2586,7 +2592,7 @@
         <v>146</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2600,7 +2606,7 @@
         <v>149</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2614,7 +2620,7 @@
         <v>152</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2628,7 +2634,7 @@
         <v>171</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2642,7 +2648,7 @@
         <v>175</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2656,7 +2662,7 @@
         <v>177</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2670,7 +2676,7 @@
         <v>179</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2684,21 +2690,21 @@
         <v>181</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>95</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2712,7 +2718,7 @@
         <v>139</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2726,7 +2732,7 @@
         <v>183</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2740,7 +2746,7 @@
         <v>185</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2754,7 +2760,7 @@
         <v>187</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2768,7 +2774,7 @@
         <v>190</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2782,7 +2788,7 @@
         <v>192</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2796,636 +2802,644 @@
         <v>195</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>196</v>
+        <v>435</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>197</v>
+        <v>436</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>397</v>
+        <v>437</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>396</v>
+        <v>438</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>296</v>
+        <v>221</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>296</v>
+        <v>220</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>297</v>
+        <v>219</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>225</v>
+        <v>298</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>225</v>
+        <v>299</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>226</v>
+        <v>300</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>304</v>
+        <v>238</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>305</v>
+        <v>239</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>306</v>
+        <v>240</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>244</v>
+        <v>301</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>245</v>
+        <v>302</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>246</v>
+        <v>303</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C111" s="2" t="s">
+      <c r="B113" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>311</v>
+        <v>291</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>433</v>
+        <v>292</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>322</v>
+        <v>316</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>438</v>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "Waypoint" to LE translations.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251A6008-6540-445F-9852-48FA855F7E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD90FB1A-4DA1-4B8F-8117-81F84F8C3320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="443">
   <si>
     <t>ID</t>
   </si>
@@ -1357,6 +1357,12 @@
   </si>
   <si>
     <t>+ Añadir Waypoint de Sierra</t>
+  </si>
+  <si>
+    <t>object.WAYPOINT</t>
+  </si>
+  <si>
+    <t>Waypoint</t>
   </si>
 </sst>
 </file>
@@ -1756,10 +1762,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,1072 +2379,1083 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>69</v>
+        <v>441</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>69</v>
+        <v>442</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>365</v>
+        <v>442</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>369</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>378</v>
+        <v>329</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C68" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>437</v>
+        <v>193</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>393</v>
+        <v>438</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>293</v>
+        <v>221</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>293</v>
+        <v>220</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>294</v>
+        <v>219</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>222</v>
+        <v>298</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>222</v>
+        <v>299</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>223</v>
+        <v>300</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>301</v>
+        <v>238</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>302</v>
+        <v>239</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>303</v>
+        <v>240</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>242</v>
+        <v>302</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>243</v>
+        <v>303</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D112" s="2" t="s">
+      <c r="D113" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
+    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+    <row r="116" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D121" s="2" t="s">
+      <c r="D122" s="2" t="s">
         <v>434</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added taser and jetpack, note that these need to be added into the sheets and taser can't set the ammo to desired one, but they're here!
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\c#\FrSLE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD90FB1A-4DA1-4B8F-8117-81F84F8C3320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1378BDF4-7818-4565-A015-E964C99A3E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15900" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="449">
   <si>
     <t>ID</t>
   </si>
@@ -1363,6 +1363,24 @@
   </si>
   <si>
     <t>Waypoint</t>
+  </si>
+  <si>
+    <t>object.JETPACK</t>
+  </si>
+  <si>
+    <t>Jetpack</t>
+  </si>
+  <si>
+    <t>Ранець</t>
+  </si>
+  <si>
+    <t>events.OnPickup</t>
+  </si>
+  <si>
+    <t>On Pickup</t>
+  </si>
+  <si>
+    <t>При піднятті</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1467,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1465,9 +1483,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема &quot;Office 2013 – 2022&quot;">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1505,7 +1523,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1611,7 +1629,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1753,7 +1771,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1762,13 +1780,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" style="2" customWidth="1"/>
     <col min="2" max="4" width="45.7109375" style="2" customWidth="1"/>
@@ -2390,1072 +2408,1094 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>69</v>
+        <v>443</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>101</v>
+        <v>444</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>365</v>
+        <v>445</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>369</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>164</v>
+        <v>446</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>166</v>
+        <v>447</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>373</v>
+        <v>448</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>244</v>
+        <v>178</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>244</v>
+        <v>178</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>140</v>
+        <v>180</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>183</v>
+        <v>244</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>184</v>
+        <v>138</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>437</v>
+        <v>191</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>440</v>
+        <v>193</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>393</v>
+        <v>435</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>394</v>
+        <v>438</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>293</v>
+        <v>217</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>294</v>
+        <v>218</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>295</v>
+        <v>221</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>296</v>
+        <v>220</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>297</v>
+        <v>219</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>222</v>
+        <v>295</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>222</v>
+        <v>296</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>223</v>
+        <v>297</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>224</v>
+        <v>298</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>225</v>
+        <v>299</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>226</v>
+        <v>300</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>301</v>
+        <v>235</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>302</v>
+        <v>236</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>303</v>
+        <v>237</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>245</v>
+        <v>301</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>253</v>
+        <v>302</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="D115" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+    <row r="117" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="118" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B124" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D122" s="2" t="s">
+      <c r="D124" s="2" t="s">
         <v>434</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Taser and fixed it.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\c#\FrSLE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1378BDF4-7818-4565-A015-E964C99A3E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CD7D41-54CB-4DF7-8FA7-284F7D4A453E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15900" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="453">
   <si>
     <t>ID</t>
   </si>
@@ -1381,6 +1381,18 @@
   </si>
   <si>
     <t>При піднятті</t>
+  </si>
+  <si>
+    <t>Ammo</t>
+  </si>
+  <si>
+    <t>InfiniteTaser</t>
+  </si>
+  <si>
+    <t>Infinite Taser</t>
+  </si>
+  <si>
+    <t>Бескінечний тазер</t>
   </si>
 </sst>
 </file>
@@ -1780,10 +1792,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3499,6 +3511,28 @@
         <v>434</v>
       </c>
     </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
taser, arrows, other things
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\c#\FrSLE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CD7D41-54CB-4DF7-8FA7-284F7D4A453E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D19210-5757-4334-B0DE-0485126562D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15900" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="459">
   <si>
     <t>ID</t>
   </si>
@@ -1393,6 +1393,24 @@
   </si>
   <si>
     <t>Бескінечний тазер</t>
+  </si>
+  <si>
+    <t>object.ARROW</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>Стрілка</t>
+  </si>
+  <si>
+    <t>object.GUN</t>
+  </si>
+  <si>
+    <t>Taser</t>
+  </si>
+  <si>
+    <t>Тазер</t>
   </si>
 </sst>
 </file>
@@ -1792,10 +1810,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2431,1105 +2449,1127 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>69</v>
+        <v>453</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>101</v>
+        <v>454</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>365</v>
+        <v>455</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>105</v>
+        <v>456</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>102</v>
+        <v>457</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>366</v>
+        <v>458</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>111</v>
+        <v>3</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>446</v>
+        <v>117</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>447</v>
+        <v>119</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>448</v>
+        <v>370</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>164</v>
+        <v>446</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>166</v>
+        <v>447</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>373</v>
+        <v>448</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>244</v>
+        <v>178</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>244</v>
+        <v>178</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>140</v>
+        <v>180</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>183</v>
+        <v>244</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>184</v>
+        <v>138</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>437</v>
+        <v>191</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>440</v>
+        <v>193</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>393</v>
+        <v>435</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>394</v>
+        <v>438</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>293</v>
+        <v>217</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>294</v>
+        <v>218</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>295</v>
+        <v>221</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>296</v>
+        <v>220</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>297</v>
+        <v>219</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>222</v>
+        <v>295</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>222</v>
+        <v>296</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>223</v>
+        <v>297</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>224</v>
+        <v>298</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>225</v>
+        <v>299</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>226</v>
+        <v>300</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>301</v>
+        <v>235</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>302</v>
+        <v>236</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>303</v>
+        <v>237</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>245</v>
+        <v>301</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>253</v>
+        <v>302</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D117" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+    <row r="119" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+    <row r="120" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>314</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>449</v>
+        <v>318</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>449</v>
+        <v>319</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>346</v>
+        <v>433</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="D126" s="2" t="s">
+      <c r="D128" s="2" t="s">
         <v>452</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Filled the empty cells in spanish translations.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Codes\c#\FrSLE\Translations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D19210-5757-4334-B0DE-0485126562D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7E189A-17CA-480B-80EB-206716EFA0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15900" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="465">
   <si>
     <t>ID</t>
   </si>
@@ -1411,6 +1411,24 @@
   </si>
   <si>
     <t>Тазер</t>
+  </si>
+  <si>
+    <t>Flecha</t>
+  </si>
+  <si>
+    <t>Al Recoger</t>
+  </si>
+  <si>
+    <t>¿Rotar?</t>
+  </si>
+  <si>
+    <t>Velocidad de Rotación</t>
+  </si>
+  <si>
+    <t>Munición</t>
+  </si>
+  <si>
+    <t>Taser infinito</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1515,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1513,9 +1531,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема &quot;Office 2013 – 2022&quot;">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013–2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1553,7 +1571,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013–2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1659,7 +1677,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013–2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1801,7 +1819,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1812,11 +1830,11 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" style="2" customWidth="1"/>
     <col min="2" max="4" width="45.7109375" style="2" customWidth="1"/>
@@ -2443,6 +2461,9 @@
       <c r="B45" s="2" t="s">
         <v>444</v>
       </c>
+      <c r="C45" s="2" t="s">
+        <v>444</v>
+      </c>
       <c r="D45" s="2" t="s">
         <v>445</v>
       </c>
@@ -2454,6 +2475,9 @@
       <c r="B46" s="2" t="s">
         <v>454</v>
       </c>
+      <c r="C46" s="2" t="s">
+        <v>459</v>
+      </c>
       <c r="D46" s="2" t="s">
         <v>455</v>
       </c>
@@ -2465,6 +2489,9 @@
       <c r="B47" s="2" t="s">
         <v>457</v>
       </c>
+      <c r="C47" s="2" t="s">
+        <v>457</v>
+      </c>
       <c r="D47" s="2" t="s">
         <v>458</v>
       </c>
@@ -2553,7 +2580,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>114</v>
       </c>
@@ -2602,6 +2629,9 @@
       <c r="B57" s="2" t="s">
         <v>447</v>
       </c>
+      <c r="C57" s="2" t="s">
+        <v>460</v>
+      </c>
       <c r="D57" s="2" t="s">
         <v>448</v>
       </c>
@@ -3536,6 +3566,9 @@
       <c r="B125" s="2" t="s">
         <v>319</v>
       </c>
+      <c r="C125" s="2" t="s">
+        <v>461</v>
+      </c>
       <c r="D125" s="2" t="s">
         <v>433</v>
       </c>
@@ -3547,6 +3580,9 @@
       <c r="B126" s="2" t="s">
         <v>321</v>
       </c>
+      <c r="C126" s="2" t="s">
+        <v>462</v>
+      </c>
       <c r="D126" s="2" t="s">
         <v>434</v>
       </c>
@@ -3558,6 +3594,9 @@
       <c r="B127" s="2" t="s">
         <v>449</v>
       </c>
+      <c r="C127" s="2" t="s">
+        <v>463</v>
+      </c>
       <c r="D127" s="2" t="s">
         <v>346</v>
       </c>
@@ -3568,6 +3607,9 @@
       </c>
       <c r="B128" s="2" t="s">
         <v>451</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>464</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>452</v>

</xml_diff>

<commit_message>
Added translations for moving platforms.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7E189A-17CA-480B-80EB-206716EFA0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0073D950-3CBC-4AA0-8DF0-57F795D4D295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="471">
   <si>
     <t>ID</t>
   </si>
@@ -1429,6 +1429,24 @@
   </si>
   <si>
     <t>Taser infinito</t>
+  </si>
+  <si>
+    <t>object.MOVING_PLATFORM</t>
+  </si>
+  <si>
+    <t>Moving Platform</t>
+  </si>
+  <si>
+    <t>Plataforma Movil</t>
+  </si>
+  <si>
+    <t>object.MOVING_PLATFORM_WAYPOINT</t>
+  </si>
+  <si>
+    <t>Moving Platform  Waypoint</t>
+  </si>
+  <si>
+    <t>Waypoint de Plataforma Movil</t>
   </si>
 </sst>
 </file>
@@ -1828,15 +1846,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="37" style="2" customWidth="1"/>
     <col min="2" max="4" width="45.7109375" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
@@ -2498,1120 +2516,1142 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>69</v>
+        <v>465</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>69</v>
+        <v>466</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>365</v>
+        <v>467</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>105</v>
+        <v>468</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>2</v>
+        <v>469</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>366</v>
+        <v>470</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>111</v>
+        <v>3</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>446</v>
+        <v>117</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>447</v>
+        <v>119</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>460</v>
+        <v>120</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>448</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>164</v>
+        <v>446</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>165</v>
+        <v>447</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>166</v>
+        <v>460</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>373</v>
+        <v>448</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>244</v>
+        <v>178</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>244</v>
+        <v>178</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>140</v>
+        <v>180</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>183</v>
+        <v>244</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>183</v>
+        <v>95</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>184</v>
+        <v>138</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>437</v>
+        <v>191</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>440</v>
+        <v>193</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>393</v>
+        <v>435</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>394</v>
+        <v>438</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>293</v>
+        <v>217</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>294</v>
+        <v>218</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>295</v>
+        <v>221</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>296</v>
+        <v>220</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>297</v>
+        <v>219</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>222</v>
+        <v>295</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>222</v>
+        <v>296</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>223</v>
+        <v>297</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>224</v>
+        <v>298</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>225</v>
+        <v>299</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>226</v>
+        <v>300</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>301</v>
+        <v>235</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>302</v>
+        <v>236</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>303</v>
+        <v>237</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>245</v>
+        <v>301</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>253</v>
+        <v>302</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="D119" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+    <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+    <row r="121" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="122" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>461</v>
+        <v>314</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>462</v>
+        <v>317</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>449</v>
+        <v>318</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>449</v>
+        <v>319</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>346</v>
+        <v>433</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B130" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C130" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="D128" s="2" t="s">
+      <c r="D130" s="2" t="s">
         <v>452</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Crows to Translations.
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0073D950-3CBC-4AA0-8DF0-57F795D4D295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22D27F0-38DE-4581-A502-C1BAAFA40D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="474">
   <si>
     <t>ID</t>
   </si>
@@ -1447,6 +1447,15 @@
   </si>
   <si>
     <t>Waypoint de Plataforma Movil</t>
+  </si>
+  <si>
+    <t>object.CROW</t>
+  </si>
+  <si>
+    <t>Crow</t>
+  </si>
+  <si>
+    <t>Cuervo</t>
   </si>
 </sst>
 </file>
@@ -1846,10 +1855,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D130"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2538,1120 +2547,1131 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>69</v>
+        <v>471</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>69</v>
+        <v>472</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>365</v>
+        <v>473</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>111</v>
+        <v>4</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>446</v>
+        <v>118</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>447</v>
+        <v>122</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>460</v>
+        <v>121</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>448</v>
+        <v>371</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>154</v>
+        <v>446</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>155</v>
+        <v>447</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>156</v>
+        <v>460</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>372</v>
+        <v>448</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>378</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>437</v>
+        <v>193</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>393</v>
+        <v>438</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>293</v>
+        <v>221</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>293</v>
+        <v>220</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>294</v>
+        <v>219</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>222</v>
+        <v>298</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>222</v>
+        <v>299</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>223</v>
+        <v>300</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>301</v>
+        <v>238</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>302</v>
+        <v>239</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>303</v>
+        <v>240</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>242</v>
+        <v>302</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>243</v>
+        <v>303</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C120" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="D120" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+    <row r="122" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>461</v>
+        <v>317</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>449</v>
+        <v>320</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>449</v>
+        <v>321</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>346</v>
+        <v>434</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C131" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="D130" s="2" t="s">
+      <c r="D131" s="2" t="s">
         <v>452</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added translations for the missing words without translation (duh)
</commit_message>
<xml_diff>
--- a/Translations/Translations.xlsx
+++ b/Translations/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\MelonLoader\FS_LevelEditor\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22D27F0-38DE-4581-A502-C1BAAFA40D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C7A83E-5509-4020-9352-7F868F992264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5C22481-FF1A-482C-BF7E-EB5A7718AF49}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="512">
   <si>
     <t>ID</t>
   </si>
@@ -1456,6 +1456,120 @@
   </si>
   <si>
     <t>Cuervo</t>
+  </si>
+  <si>
+    <t>AddMovingPlatformWaypoint</t>
+  </si>
+  <si>
+    <t>+ Add Platform Waypoint</t>
+  </si>
+  <si>
+    <t>+ Añadir Waypoint de Plataforma</t>
+  </si>
+  <si>
+    <t>InvisibleEdges</t>
+  </si>
+  <si>
+    <t>Invisible Edges</t>
+  </si>
+  <si>
+    <t>Border Invisibles</t>
+  </si>
+  <si>
+    <t>StartMovingAtStart</t>
+  </si>
+  <si>
+    <t>Start Moving At Start</t>
+  </si>
+  <si>
+    <t>Mover Al Inicio</t>
+  </si>
+  <si>
+    <t>MovingSpeed</t>
+  </si>
+  <si>
+    <t>Moving Speed</t>
+  </si>
+  <si>
+    <t>Velocidad de Movimiento</t>
+  </si>
+  <si>
+    <t>StartDelay</t>
+  </si>
+  <si>
+    <t>Start Delay</t>
+  </si>
+  <si>
+    <t>Espera al Inicio</t>
+  </si>
+  <si>
+    <t>MovementMode</t>
+  </si>
+  <si>
+    <t>Movement Mode</t>
+  </si>
+  <si>
+    <t>Modo de Movimiento</t>
+  </si>
+  <si>
+    <t>None_Mayus</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>NINGUNO</t>
+  </si>
+  <si>
+    <t>TravelBack_Mayus</t>
+  </si>
+  <si>
+    <t>TRAVEL BACK</t>
+  </si>
+  <si>
+    <t>REGRESARSE</t>
+  </si>
+  <si>
+    <t>Loop_Mayus</t>
+  </si>
+  <si>
+    <t>LOOP</t>
+  </si>
+  <si>
+    <t>BUCLE</t>
+  </si>
+  <si>
+    <t>IsAutomatic</t>
+  </si>
+  <si>
+    <t>Is Automatic?</t>
+  </si>
+  <si>
+    <t>¿Es Automática?</t>
+  </si>
+  <si>
+    <t>CLOSED</t>
+  </si>
+  <si>
+    <t>CERRADA</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>ABIERTA</t>
+  </si>
+  <si>
+    <t>LOCKED</t>
+  </si>
+  <si>
+    <t>BLOQUEADA</t>
+  </si>
+  <si>
+    <t>UNLOCKED</t>
+  </si>
+  <si>
+    <t>DESBLOQUEADA</t>
   </si>
 </sst>
 </file>
@@ -1855,10 +1969,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6961A5F-F8EA-4989-8112-A0ACE51D011E}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,651 +3142,805 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>393</v>
+        <v>474</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>293</v>
+        <v>221</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>293</v>
+        <v>220</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>294</v>
+        <v>219</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>222</v>
+        <v>298</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>222</v>
+        <v>299</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>223</v>
+        <v>300</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>301</v>
+        <v>238</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>302</v>
+        <v>239</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>303</v>
+        <v>240</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>242</v>
+        <v>302</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>243</v>
+        <v>303</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D121" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+    <row r="122" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C122" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C123" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="124" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B124" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>292</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>461</v>
+        <v>317</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>449</v>
+        <v>320</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>449</v>
+        <v>321</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>346</v>
+        <v>434</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C132" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="D132" s="2" t="s">
         <v>452</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>